<commit_message>
Update of column changes
</commit_message>
<xml_diff>
--- a/supplier csv analysis.xlsx
+++ b/supplier csv analysis.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E10" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -115,30 +115,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Difference between Entity and Stock Quantity?</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -271,9 +247,6 @@
 Estimated Time of Arrival</t>
   </si>
   <si>
-    <t>Entity - quantity</t>
-  </si>
-  <si>
     <t>Gcode  - supplier internal code</t>
   </si>
   <si>
@@ -311,6 +284,9 @@
   </si>
   <si>
     <t>items ignored</t>
+  </si>
+  <si>
+    <t>Entity</t>
   </si>
 </sst>
 </file>
@@ -391,7 +367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -638,10 +614,62 @@
       <right style="dashed">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="hair">
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -650,13 +678,43 @@
       <left style="dashed">
         <color auto="1"/>
       </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -665,55 +723,40 @@
       <left style="dashed">
         <color auto="1"/>
       </left>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
+      <top style="dotted">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -726,7 +769,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -740,12 +783,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -758,25 +795,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -795,58 +856,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1152,7 +1213,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G34"/>
+  <dimension ref="B1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1170,159 +1231,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="10" t="s">
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="27"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="27"/>
+      <c r="C5" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="27"/>
+      <c r="C6" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="27"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
-      <c r="C5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14" t="s">
-        <v>11</v>
-      </c>
+      <c r="F7" s="45"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="45"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="28"/>
+      <c r="C9" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>8</v>
+      <c r="F11" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-      <c r="C13" s="24" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="32"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1332,15 +1395,15 @@
         <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
-      <c r="C15" s="39" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" s="23" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="3"/>
@@ -1348,169 +1411,160 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="17"/>
+      <c r="F16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="23"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-      <c r="C19" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="32"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="33"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="23"/>
-      <c r="C21" s="29" t="s">
+      <c r="B21" s="31"/>
+      <c r="C21" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="31" t="s">
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="17" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="23"/>
-      <c r="C22" s="29" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="31" t="s">
-        <v>42</v>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="23"/>
-      <c r="C23" s="29" t="s">
+      <c r="B23" s="31"/>
+      <c r="C23" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="34"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="23"/>
-      <c r="C24" s="29" t="s">
+      <c r="B24" s="31"/>
+      <c r="C24" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="34"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="20"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="23"/>
-      <c r="C25" s="29" t="s">
+      <c r="B25" s="31"/>
+      <c r="C25" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="34"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
-      <c r="C26" s="29" t="s">
+      <c r="B26" s="31"/>
+      <c r="C26" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="34"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
-      <c r="C27" s="29" t="s">
+      <c r="B27" s="31"/>
+      <c r="C27" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="34"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="23"/>
-      <c r="C28" s="29" t="s">
+      <c r="B28" s="31"/>
+      <c r="C28" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="34"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="20"/>
     </row>
     <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="23"/>
-      <c r="C29" s="29" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="34"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
-      <c r="C30" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="40"/>
-      <c r="C33" s="42" t="s">
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="24"/>
+      <c r="C32" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="25"/>
+      <c r="C33" t="s">
         <v>53</v>
-      </c>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="41"/>
-      <c r="C34" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B19"/>
-    <mergeCell ref="B20:B30"/>
-    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="B20:B29"/>
+    <mergeCell ref="C32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>